<commit_message>
baseline shooting analysis and results
</commit_message>
<xml_diff>
--- a/Bionic Shooter Range Tests/ShooterTest-Range.xlsx
+++ b/Bionic Shooter Range Tests/ShooterTest-Range.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanroorda/Dropbox/FTC/FTC 2025-2026/Shooter Data/Datalogs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Desktop\FTC\2025-2026 Decode\Decode-Data-Analysis-2025-2026\Bionic Shooter Range Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0A5668E-84D3-424F-854D-60CCBC0BF9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="6260" windowWidth="36000" windowHeight="23380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26520" yWindow="6255" windowWidth="36000" windowHeight="23385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="One at a Time" sheetId="2" r:id="rId1"/>
+    <sheet name="One at a Time (2)" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="24">
   <si>
     <t>Power</t>
   </si>
@@ -118,12 +118,18 @@
   <si>
     <t>Dist = 2</t>
   </si>
+  <si>
+    <t>Hit</t>
+  </si>
+  <si>
+    <t>Missed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -162,6 +168,13 @@
       <b/>
       <sz val="10"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -244,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -286,11 +299,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="69">
     <dxf>
       <font>
         <b/>
@@ -376,6 +390,90 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF6F8F9"/>
@@ -833,100 +931,100 @@
     </dxf>
   </dxfs>
   <tableStyles count="19">
-    <tableStyle name="One at a Time-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="One at a Time-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="68"/>
+      <tableStyleElement type="firstRowStripe" dxfId="67"/>
+      <tableStyleElement type="secondRowStripe" dxfId="66"/>
+    </tableStyle>
+    <tableStyle name="One at a Time-style 2" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="65"/>
+      <tableStyleElement type="firstRowStripe" dxfId="64"/>
+      <tableStyleElement type="secondRowStripe" dxfId="63"/>
+    </tableStyle>
+    <tableStyle name="One at a Time-style 3" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="62"/>
       <tableStyleElement type="firstRowStripe" dxfId="61"/>
       <tableStyleElement type="secondRowStripe" dxfId="60"/>
     </tableStyle>
-    <tableStyle name="One at a Time-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="One at a Time-style 4" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="59"/>
       <tableStyleElement type="firstRowStripe" dxfId="58"/>
       <tableStyleElement type="secondRowStripe" dxfId="57"/>
     </tableStyle>
-    <tableStyle name="One at a Time-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
+    <tableStyle name="One at a Time-style 5" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="56"/>
       <tableStyleElement type="firstRowStripe" dxfId="55"/>
       <tableStyleElement type="secondRowStripe" dxfId="54"/>
     </tableStyle>
-    <tableStyle name="One at a Time-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
+    <tableStyle name="One at a Time-style 6" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="53"/>
       <tableStyleElement type="firstRowStripe" dxfId="52"/>
       <tableStyleElement type="secondRowStripe" dxfId="51"/>
     </tableStyle>
-    <tableStyle name="One at a Time-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
+    <tableStyle name="One at a Time-style 7" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="50"/>
       <tableStyleElement type="firstRowStripe" dxfId="49"/>
       <tableStyleElement type="secondRowStripe" dxfId="48"/>
     </tableStyle>
-    <tableStyle name="One at a Time-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
+    <tableStyle name="3 Rapidly-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="47"/>
       <tableStyleElement type="firstRowStripe" dxfId="46"/>
       <tableStyleElement type="secondRowStripe" dxfId="45"/>
     </tableStyle>
-    <tableStyle name="One at a Time-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
+    <tableStyle name="3 Rapidly-style 2" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="44"/>
       <tableStyleElement type="firstRowStripe" dxfId="43"/>
       <tableStyleElement type="secondRowStripe" dxfId="42"/>
     </tableStyle>
-    <tableStyle name="3 Rapidly-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
+    <tableStyle name="3 Rapidly-style 3" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="41"/>
       <tableStyleElement type="firstRowStripe" dxfId="40"/>
       <tableStyleElement type="secondRowStripe" dxfId="39"/>
     </tableStyle>
-    <tableStyle name="3 Rapidly-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
+    <tableStyle name="3 Rapidly-style 4" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="38"/>
       <tableStyleElement type="firstRowStripe" dxfId="37"/>
       <tableStyleElement type="secondRowStripe" dxfId="36"/>
     </tableStyle>
-    <tableStyle name="3 Rapidly-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
+    <tableStyle name="3 Rapidly-style 5" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="35"/>
       <tableStyleElement type="firstRowStripe" dxfId="34"/>
       <tableStyleElement type="secondRowStripe" dxfId="33"/>
     </tableStyle>
-    <tableStyle name="3 Rapidly-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0A000000}">
+    <tableStyle name="3 Rapidly-style 6" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="32"/>
       <tableStyleElement type="firstRowStripe" dxfId="31"/>
       <tableStyleElement type="secondRowStripe" dxfId="30"/>
     </tableStyle>
-    <tableStyle name="3 Rapidly-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0B000000}">
+    <tableStyle name="3 Rapidly-style 7" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="29"/>
       <tableStyleElement type="firstRowStripe" dxfId="28"/>
       <tableStyleElement type="secondRowStripe" dxfId="27"/>
     </tableStyle>
-    <tableStyle name="3 Rapidly-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0C000000}">
+    <tableStyle name="3 Rapidly-style 8" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="26"/>
       <tableStyleElement type="firstRowStripe" dxfId="25"/>
       <tableStyleElement type="secondRowStripe" dxfId="24"/>
     </tableStyle>
-    <tableStyle name="3 Rapidly-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0D000000}">
+    <tableStyle name="3 Rapidly-style 9" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="23"/>
       <tableStyleElement type="firstRowStripe" dxfId="22"/>
       <tableStyleElement type="secondRowStripe" dxfId="21"/>
     </tableStyle>
-    <tableStyle name="3 Rapidly-style 8" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0E000000}">
+    <tableStyle name="3 Rapidly-style 10" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="20"/>
       <tableStyleElement type="firstRowStripe" dxfId="19"/>
       <tableStyleElement type="secondRowStripe" dxfId="18"/>
     </tableStyle>
-    <tableStyle name="3 Rapidly-style 9" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0F000000}">
+    <tableStyle name="3 Rapidly-style 11" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="17"/>
       <tableStyleElement type="firstRowStripe" dxfId="16"/>
       <tableStyleElement type="secondRowStripe" dxfId="15"/>
     </tableStyle>
-    <tableStyle name="3 Rapidly-style 10" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF10000000}">
+    <tableStyle name="3 Rapidly-style 12" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="14"/>
       <tableStyleElement type="firstRowStripe" dxfId="13"/>
       <tableStyleElement type="secondRowStripe" dxfId="12"/>
-    </tableStyle>
-    <tableStyle name="3 Rapidly-style 11" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF11000000}">
-      <tableStyleElement type="headerRow" dxfId="11"/>
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
-      <tableStyleElement type="secondRowStripe" dxfId="9"/>
-    </tableStyle>
-    <tableStyle name="3 Rapidly-style 12" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF12000000}">
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -940,81 +1038,1618 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'One at a Time (2)'!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'One at a Time (2)'!$K$3:$P$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'One at a Time (2)'!$K$4:$P$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-5C02-482A-AD34-72C2EE17DCB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'One at a Time (2)'!$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'One at a Time (2)'!$K$5:$P$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-5C02-482A-AD34-72C2EE17DCB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'One at a Time (2)'!$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'One at a Time (2)'!$K$6:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-5C02-482A-AD34-72C2EE17DCB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'One at a Time (2)'!$J$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.65</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'One at a Time (2)'!$K$7:$P$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-5C02-482A-AD34-72C2EE17DCB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'One at a Time (2)'!$J$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'One at a Time (2)'!$K$8:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-5C02-482A-AD34-72C2EE17DCB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'One at a Time (2)'!$J$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'One at a Time (2)'!$K$9:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-5C02-482A-AD34-72C2EE17DCB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'One at a Time (2)'!$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'One at a Time (2)'!$K$10:$P$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-5C02-482A-AD34-72C2EE17DCB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'One at a Time (2)'!$J$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'One at a Time (2)'!$K$12:$P$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-5C02-482A-AD34-72C2EE17DCB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'One at a Time (2)'!$J$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'One at a Time (2)'!$K$13:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-5C02-482A-AD34-72C2EE17DCB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="612549568"/>
+        <c:axId val="612552480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="612549568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (ft)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="612552480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="612552480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number scored</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="612549568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Dist14" displayName="Dist14" ref="A2:E10" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Dist14" displayName="Dist14" ref="A2:E10" headerRowDxfId="11">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Power"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ball #1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ball #2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Ball #3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Timestamp"/>
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Ball #3"/>
+    <tableColumn id="5" name="Timestamp"/>
   </tableColumns>
   <tableStyleInfo name="3 Rapidly-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Dist611" displayName="Dist611" ref="A49:E55" headerRowDxfId="2">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Ball #3"/>
+    <tableColumn id="5" name="Timestamp"/>
+  </tableColumns>
+  <tableStyleInfo name="One at a Time-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Dist412" displayName="Dist412" ref="A59:E66" headerRowDxfId="1">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Ball #3"/>
+    <tableColumn id="5" name="Timestamp"/>
+  </tableColumns>
+  <tableStyleInfo name="One at a Time-style 6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Dist213" displayName="Dist213" ref="A70:E76" headerRowDxfId="0">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Ball #3"/>
+    <tableColumn id="5" name="Timestamp"/>
+  </tableColumns>
+  <tableStyleInfo name="One at a Time-style 7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Dist12" displayName="Dist12" ref="A14:E24" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Dist12" displayName="Dist12" ref="A14:E24" headerRowDxfId="10">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Power"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Ball #1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ball #2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Ball #3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Timestamp"/>
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Ball #3"/>
+    <tableColumn id="5" name="Timestamp"/>
   </tableColumns>
   <tableStyleInfo name="One at a Time-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Dist10" displayName="Dist10" ref="A28:E36" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Dist10" displayName="Dist10" ref="A28:E36" headerRowDxfId="9">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Power"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Ball #1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Ball #2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Column 4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Timestamp"/>
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Column 4"/>
+    <tableColumn id="5" name="Timestamp"/>
   </tableColumns>
   <tableStyleInfo name="One at a Time-style 3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Dist6" displayName="Dist6" ref="A49:E55" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Dist6" displayName="Dist6" ref="A49:E55" headerRowDxfId="8">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Ball #1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Ball #2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Ball #3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Timestamp"/>
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Ball #3"/>
+    <tableColumn id="5" name="Timestamp"/>
   </tableColumns>
   <tableStyleInfo name="One at a Time-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Dist4" displayName="Dist4" ref="A59:E66" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Dist4" displayName="Dist4" ref="A59:E66" headerRowDxfId="7">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Power"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Ball #1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Ball #2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Ball #3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Timestamp"/>
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Ball #3"/>
+    <tableColumn id="5" name="Timestamp"/>
   </tableColumns>
   <tableStyleInfo name="One at a Time-style 6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Dist2" displayName="Dist2" ref="A70:E76" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Dist2" displayName="Dist2" ref="A70:E76" headerRowDxfId="6">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Power"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Ball #1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Ball #2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Ball #3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Timestamp"/>
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Ball #3"/>
+    <tableColumn id="5" name="Timestamp"/>
   </tableColumns>
   <tableStyleInfo name="One at a Time-style 7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Dist145" displayName="Dist145" ref="A2:E10" headerRowDxfId="5">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Ball #3"/>
+    <tableColumn id="5" name="Timestamp"/>
+  </tableColumns>
+  <tableStyleInfo name="3 Rapidly-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Dist129" displayName="Dist129" ref="A14:E24" headerRowDxfId="4">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Ball #3"/>
+    <tableColumn id="5" name="Timestamp"/>
+  </tableColumns>
+  <tableStyleInfo name="One at a Time-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Dist1010" displayName="Dist1010" ref="A28:E36" headerRowDxfId="3">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Power"/>
+    <tableColumn id="2" name="Ball #1"/>
+    <tableColumn id="3" name="Ball #2"/>
+    <tableColumn id="4" name="Column 4"/>
+    <tableColumn id="5" name="Timestamp"/>
+  </tableColumns>
+  <tableStyleInfo name="One at a Time-style 3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1215,36 +2850,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="7" max="9" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="13" max="15" width="15.6640625" customWidth="1"/>
-    <col min="16" max="16" width="11.5" customWidth="1"/>
-    <col min="18" max="19" width="15.6640625" customWidth="1"/>
-    <col min="20" max="20" width="11.5" customWidth="1"/>
-    <col min="23" max="25" width="15.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.5" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="7" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="13" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="18" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="23" max="25" width="15.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1261,12 +2899,16 @@
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2"/>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>17.75</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>0.5</v>
       </c>
@@ -1275,16 +2917,13 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="G3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4">
-        <v>17.75</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>0.6</v>
       </c>
@@ -1293,13 +2932,13 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="G4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>0.7</v>
       </c>
@@ -1315,11 +2954,13 @@
       <c r="E5" s="9">
         <v>153953</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>0.75</v>
       </c>
@@ -1335,8 +2976,11 @@
       <c r="E6" s="9">
         <v>170336</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>0.8</v>
       </c>
@@ -1352,8 +2996,11 @@
       <c r="E7" s="9">
         <v>153622</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>0.85</v>
       </c>
@@ -1369,8 +3016,11 @@
       <c r="E8" s="9">
         <v>170158</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>0.9</v>
       </c>
@@ -1386,8 +3036,11 @@
       <c r="E9" s="9">
         <v>153342</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>1</v>
       </c>
@@ -1403,25 +3056,28 @@
       <c r="E10" s="9">
         <v>153007</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L12" s="1"/>
       <c r="M12" s="4"/>
       <c r="V12" s="1"/>
       <c r="W12" s="4"/>
     </row>
-    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
       <c r="L13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
@@ -1438,7 +3094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>0.5</v>
       </c>
@@ -1447,7 +3103,7 @@
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>0.6</v>
       </c>
@@ -1462,6 +3118,9 @@
       </c>
       <c r="E16" s="9">
         <v>155330</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1471,7 +3130,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>0.7</v>
       </c>
@@ -1487,7 +3146,9 @@
       <c r="E17" s="9">
         <v>155136</v>
       </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1496,7 +3157,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>0.75</v>
       </c>
@@ -1512,7 +3173,9 @@
       <c r="E18" s="9">
         <v>165026</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2">
+        <v>2</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1521,7 +3184,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>0.8</v>
       </c>
@@ -1537,7 +3200,9 @@
       <c r="E19" s="9">
         <v>154958</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1546,7 +3211,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>0.85</v>
       </c>
@@ -1562,7 +3227,9 @@
       <c r="E20" s="9">
         <v>164523</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1571,7 +3238,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>0.85</v>
       </c>
@@ -1587,7 +3254,9 @@
       <c r="E21" s="9">
         <v>164735</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2">
+        <v>3</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1596,7 +3265,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>0.9</v>
       </c>
@@ -1610,7 +3279,9 @@
         <v>8</v>
       </c>
       <c r="E22" s="9"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1619,7 +3290,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
         <v>0.9</v>
       </c>
@@ -1635,12 +3306,14 @@
       <c r="E23" s="14">
         <v>154813</v>
       </c>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>1</v>
       </c>
@@ -1656,25 +3329,27 @@
       <c r="E24" s="15">
         <v>154532</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2">
+        <v>3</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>17</v>
       </c>
@@ -1687,7 +3362,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>0</v>
       </c>
@@ -1712,7 +3387,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>0.6</v>
       </c>
@@ -1728,7 +3403,9 @@
       <c r="E29" s="9">
         <v>160203</v>
       </c>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="K29" s="2"/>
@@ -1736,7 +3413,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>0.6</v>
       </c>
@@ -1752,7 +3429,9 @@
       <c r="E30" s="9">
         <v>155952</v>
       </c>
-      <c r="G30" s="2"/>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -1761,7 +3440,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>0.65</v>
       </c>
@@ -1777,7 +3456,9 @@
       <c r="E31" s="9">
         <v>164329</v>
       </c>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2">
+        <v>2</v>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -1786,7 +3467,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>0.7</v>
       </c>
@@ -1802,7 +3483,9 @@
       <c r="E32" s="9">
         <v>155847</v>
       </c>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2">
+        <v>3</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="K32" s="2"/>
@@ -1810,7 +3493,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>0.75</v>
       </c>
@@ -1826,8 +3509,11 @@
       <c r="E33" s="9">
         <v>164137</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>0.8</v>
       </c>
@@ -1843,8 +3529,11 @@
       <c r="E34" s="9">
         <v>155752</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G34" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>0.9</v>
       </c>
@@ -1860,8 +3549,11 @@
       <c r="E35" s="9">
         <v>155629</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>1</v>
       </c>
@@ -1877,13 +3569,16 @@
       <c r="E36" s="9">
         <v>155506</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
         <v>0.5</v>
       </c>
@@ -1899,8 +3594,11 @@
       <c r="E40" s="14">
         <v>160815</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>0.6</v>
       </c>
@@ -1916,8 +3614,11 @@
       <c r="E41" s="15">
         <v>160525</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <v>0.7</v>
       </c>
@@ -1933,8 +3634,11 @@
       <c r="E42" s="14">
         <v>160438</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <v>0.8</v>
       </c>
@@ -1950,8 +3654,11 @@
       <c r="E43" s="15">
         <v>160335</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="13">
         <v>0.9</v>
       </c>
@@ -1959,8 +3666,11 @@
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>1</v>
       </c>
@@ -1968,13 +3678,16 @@
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>0</v>
       </c>
@@ -1994,7 +3707,7 @@
       <c r="K49" s="6"/>
       <c r="Q49" s="6"/>
     </row>
-    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>0.5</v>
       </c>
@@ -2010,8 +3723,11 @@
       <c r="E50" s="9">
         <v>161338</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>0.6</v>
       </c>
@@ -2027,8 +3743,11 @@
       <c r="E51" s="9">
         <v>161121</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>0.7</v>
       </c>
@@ -2044,8 +3763,11 @@
       <c r="E52" s="9">
         <v>161418</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>0.8</v>
       </c>
@@ -2054,7 +3776,7 @@
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>0.9</v>
       </c>
@@ -2063,7 +3785,7 @@
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>1</v>
       </c>
@@ -2072,16 +3794,16 @@
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>0</v>
       </c>
@@ -2098,7 +3820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>0.5</v>
       </c>
@@ -2114,8 +3836,11 @@
       <c r="E60" s="9">
         <v>161618</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>0.55000000000000004</v>
       </c>
@@ -2131,8 +3856,11 @@
       <c r="E61" s="9">
         <v>163858</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>0.6</v>
       </c>
@@ -2148,8 +3876,11 @@
       <c r="E62" s="9">
         <v>161542</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>0.7</v>
       </c>
@@ -2165,8 +3896,11 @@
       <c r="E63" s="9">
         <v>161736</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>0.8</v>
       </c>
@@ -2174,8 +3908,11 @@
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
-    </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>0.9</v>
       </c>
@@ -2183,8 +3920,11 @@
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>1</v>
       </c>
@@ -2192,13 +3932,16 @@
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
-    </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
         <v>0</v>
       </c>
@@ -2215,7 +3958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
         <v>0.5</v>
       </c>
@@ -2232,7 +3975,7 @@
         <v>162232</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
         <v>0.6</v>
       </c>
@@ -2249,7 +3992,7 @@
         <v>162138</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
         <v>0.7</v>
       </c>
@@ -2266,7 +4009,7 @@
         <v>162328</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
         <v>0.8</v>
       </c>
@@ -2275,7 +4018,7 @@
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
         <v>0.9</v>
       </c>
@@ -2284,7 +4027,7 @@
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
         <v>1</v>
       </c>
@@ -2295,10 +4038,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="B71:D76 B40:D45 B50:D55 B60:D66 B3:D10 B29:D36 B15:D24" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B71:D76 B40:D45 B50:D55 B60:D66 B3:D10 B29:D36 B15:D24">
       <formula1>"Missed Short,Missed Far,Scored,Bounced Out"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A71:A76 A40:A45 A50:A55 A60:A66 A3:A10 A29:A36 A15:A24" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A71:A76 A40:A45 A50:A55 A60:A66 A3:A10 A29:A36 A15:A24">
       <formula1>AND(ISNUMBER(A3),(NOT(OR(NOT(ISERROR(DATEVALUE(A3))), AND(ISNUMBER(A3), LEFT(CELL("format", A3))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -2312,4 +4055,1439 @@
     <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:W76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="7" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="13" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="18" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="23" max="25" width="15.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>17.75</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3">
+        <v>10</v>
+      </c>
+      <c r="O3">
+        <v>12</v>
+      </c>
+      <c r="P3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4">
+        <v>0.5</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="9">
+        <v>153953</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="9">
+        <v>170336</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.6</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="9">
+        <v>153622</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>0.65</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>0.85</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9">
+        <v>170158</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>0.7</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="9">
+        <v>153342</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0.75</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>1</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9">
+        <v>153007</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>0.8</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>0.85</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>2</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2</v>
+      </c>
+      <c r="V11" s="1"/>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>0.9</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1</v>
+      </c>
+      <c r="O12" s="2">
+        <v>1</v>
+      </c>
+      <c r="P12" s="2">
+        <v>1</v>
+      </c>
+      <c r="V12" s="1"/>
+      <c r="W12" s="4"/>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>3</v>
+      </c>
+      <c r="P13" s="2">
+        <v>2</v>
+      </c>
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="17"/>
+    </row>
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="9">
+        <v>155330</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="9">
+        <v>155136</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="9">
+        <v>165026</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="9">
+        <v>154958</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>0.85</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="9">
+        <v>164523</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>0.85</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="9">
+        <v>164735</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="14">
+        <v>154813</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>1</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="15">
+        <v>154532</v>
+      </c>
+      <c r="G24" s="2">
+        <v>3</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="9">
+        <v>160203</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="9">
+        <v>155952</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="5"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="9">
+        <v>164329</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="5"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="9">
+        <v>155847</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="9">
+        <v>164137</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="9">
+        <v>155752</v>
+      </c>
+      <c r="G34" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="9">
+        <v>155629</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>1</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="9">
+        <v>155506</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="14">
+        <v>160815</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="15">
+        <v>160525</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="14">
+        <v>160438</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="15">
+        <v>160335</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="8">
+        <v>1</v>
+      </c>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="Q49" s="6"/>
+    </row>
+    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="9">
+        <v>161338</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="9">
+        <v>161121</v>
+      </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="9">
+        <v>161418</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+    </row>
+    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+    </row>
+    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="7">
+        <v>1</v>
+      </c>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+    </row>
+    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="L56" s="3"/>
+    </row>
+    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="9">
+        <v>161618</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="9">
+        <v>163858</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="9">
+        <v>161542</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="9">
+        <v>161736</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
+        <v>1</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="9">
+        <v>162232</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="9">
+        <v>162138</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="9">
+        <v>162328</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+    </row>
+    <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+    </row>
+    <row r="76" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="7">
+        <v>1</v>
+      </c>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A71:A76 A40:A45 A50:A55 A60:A66 A3:A10 A29:A36 A15:A24">
+      <formula1>AND(ISNUMBER(A3),(NOT(OR(NOT(ISERROR(DATEVALUE(A3))), AND(ISNUMBER(A3), LEFT(CELL("format", A3))="D")))))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="B71:D76 B40:D45 B50:D55 B60:D66 B3:D10 B29:D36 B15:D24">
+      <formula1>"Missed Short,Missed Far,Scored,Bounced Out"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="6">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>